<commit_message>
Added joined NBA table
</commit_message>
<xml_diff>
--- a/Resources/data/NBA from Wikipedia.xlsx
+++ b/Resources/data/NBA from Wikipedia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ae1caf55cd77bee/Desktop/School/UCI Bootcamp/Projects/NCAA_Athletic_Dept_Budgets/Resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{AF79684D-28DE-824D-AE3C-0D3B540CA292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1173D079-8AF4-425D-A7F2-4ED1AFD6904F}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{AF79684D-28DE-824D-AE3C-0D3B540CA292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{344352FB-D33F-44F5-BE3F-AE0D9B37E956}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3734B077-4F33-4644-B9D1-47C29C3C48C1}"/>
   </bookViews>
@@ -10452,7 +10452,7 @@
   <dimension ref="A1:H509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>